<commit_message>
revamped diagnostics to generalize to any table. Breaks with older versions
</commit_message>
<xml_diff>
--- a/test_data/test_table.xlsx
+++ b/test_data/test_table.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://apn01.sharepoint.com/sites/benchmarking/Shared Documents/Data Quality/Diagnostics/data_diagnostics/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_F25DC773A252ABDACC104872311C4F9E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3B4E54F-581D-40EB-9C11-F8C51AF2902A}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_F25DC773A252ABDACC104872311C4F9E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A648CBCE-096B-4FD3-9B17-3029EDA1636E}"/>
   <bookViews>
-    <workbookView xWindow="31200" yWindow="1335" windowWidth="15180" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38595" yWindow="1470" windowWidth="17325" windowHeight="14130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -97,6 +108,15 @@
   </si>
   <si>
     <t>duplicate against positive</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>sum negative</t>
+  </si>
+  <si>
+    <t>sum positive</t>
   </si>
 </sst>
 </file>
@@ -432,20 +452,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="5" width="13.81640625" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
+    <col min="6" max="7" width="21.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -465,10 +485,13 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -487,11 +510,15 @@
       <c r="F2" s="3">
         <v>45210.520833333336</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4">
+        <f>SUM(B2,D2)</f>
+        <v>25.5</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -510,11 +537,15 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G10" si="0">SUM(B3,D3)</f>
+        <v>45570</v>
+      </c>
+      <c r="H3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -533,11 +564,15 @@
       <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -556,11 +591,15 @@
       <c r="F5" s="3">
         <v>45210.520833333336</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="H5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -579,19 +618,27 @@
       <c r="F6" s="3">
         <v>45292.520833333336</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="H6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -610,11 +657,15 @@
       <c r="F8" s="3">
         <v>45210.520833333336</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>25.5</v>
+      </c>
+      <c r="H8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -633,11 +684,15 @@
       <c r="F9" s="3">
         <v>45210.520833333336</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>25.5</v>
+      </c>
+      <c r="H9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -654,8 +709,66 @@
       <c r="F10" s="3">
         <v>45210.520833333336</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>25.5</v>
+      </c>
+      <c r="H10" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>15.5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>45210</v>
+      </c>
+      <c r="F11" s="3">
+        <v>45210.520833333336</v>
+      </c>
+      <c r="G11" s="4">
+        <f>SUM(B11,D11)-5</f>
+        <v>20.5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>15.5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>45210</v>
+      </c>
+      <c r="F12" s="3">
+        <v>45210.520833333336</v>
+      </c>
+      <c r="G12" s="4">
+        <f>SUM(B12,D12)+5</f>
+        <v>30.5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>